<commit_message>
App requirements and user stories updated.
</commit_message>
<xml_diff>
--- a/src/main/resources/PetSitter/RequirementsList.xlsx
+++ b/src/main/resources/PetSitter/RequirementsList.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jp\spring-boot-openapi\src\main\resources\PetSitter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF48A78-770A-4BD0-93B7-6ABF20A08087}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19D9F0D-31E4-4ABD-B537-C72C7E5D0541}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A9D3E40F-915C-4BF8-899F-BC9B8C8FC226}"/>
+    <workbookView xWindow="-28920" yWindow="-210" windowWidth="29040" windowHeight="15840" xr2:uid="{A9D3E40F-915C-4BF8-899F-BC9B8C8FC226}"/>
   </bookViews>
   <sheets>
     <sheet name="App user roles" sheetId="2" r:id="rId1"/>
-    <sheet name="Requirements" sheetId="1" r:id="rId2"/>
-    <sheet name="User Story" sheetId="3" r:id="rId3"/>
+    <sheet name="User Stories" sheetId="3" r:id="rId2"/>
+    <sheet name="Requirements" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="65">
   <si>
     <t>Requirements list draft</t>
   </si>
@@ -102,13 +102,142 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Requirements list for next sprint</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Story description</t>
+  </si>
+  <si>
+    <t>Selected to realize</t>
+  </si>
+  <si>
+    <t>I can register a new account and choose my role, so that I can log in</t>
+  </si>
+  <si>
+    <t>I can log in to my account, so that I can use the marketplace.</t>
+  </si>
+  <si>
+    <t>I can modify my account details.</t>
+  </si>
+  <si>
+    <t>I can delete my account.</t>
+  </si>
+  <si>
+    <t>As a pet owner, I can post a job on PetSitter, including a description of one of 
+my dogs, so that pet sitters can apply.</t>
+  </si>
+  <si>
+    <t>As a pet owner, I can see a list of jobs I have posted.</t>
+  </si>
+  <si>
+    <t>As a pet owner, given that I have posted a job, I can view and modify its details.</t>
+  </si>
+  <si>
+    <t>As a pet owner, given that I have posted a job, I can delete it.</t>
+  </si>
+  <si>
+    <t>As a pet owner, given that I have posted a job, I can see the pet sitters that applied.</t>
+  </si>
+  <si>
+    <t>As a pet owner, given that I have found a suitable candidate, I can approve them.</t>
+  </si>
+  <si>
+    <t>As a pet sitter, I can view a list of pets that need looking after.</t>
+  </si>
+  <si>
+    <t>As a pet sitter, given that I have found a job, I can apply for it.</t>
+  </si>
+  <si>
+    <t>As an administrator, I can modify other users’ account details.</t>
+  </si>
+  <si>
+    <t>Project stage</t>
+  </si>
+  <si>
+    <t>Sprint II</t>
+  </si>
+  <si>
+    <t>As an administrator, I can edit jobs that other users have posted.</t>
+  </si>
+  <si>
+    <t>As an administrator, I can delete users.</t>
+  </si>
+  <si>
+    <t>Pet owners can post jobs containing one or more pets of various types.</t>
+  </si>
+  <si>
+    <t>Pet sitters can browse jobs based on certain criteria, divided into pages.</t>
+  </si>
+  <si>
+    <t>Sprint I</t>
+  </si>
+  <si>
+    <t>As a pet sitter, I can specify the kinds of jobs I’m looking for and browse jobs with those criteria.</t>
+  </si>
+  <si>
+    <t>As a pet sitter, given that I’m seeing a list of jobs and there are more jobs available, 
+I can navigate to the next page to see more jobs</t>
+  </si>
+  <si>
+    <t>As a petsitter, I can register a new account and choose my role, so that I can log in.</t>
+  </si>
+  <si>
+    <t>As a petsitter, I can log in to my account, so that I can use the marketplace.</t>
+  </si>
+  <si>
+    <t>As a petsitter, I can modify my account details.</t>
+  </si>
+  <si>
+    <t>As a petsitter, I can delete my account.</t>
+  </si>
+  <si>
+    <t>As a petowner, I can register a new account and choose my role, so that I can log in.</t>
+  </si>
+  <si>
+    <t>As a petowner, I can log in to my account, so that I can use the marketplace.</t>
+  </si>
+  <si>
+    <t>As a petowner, I can post a job on PetSitter, including a description of one of my dogs, so that
+ pet sitters can apply.</t>
+  </si>
+  <si>
+    <t>As a petowner, I can see a list of jobs I have posted.</t>
+  </si>
+  <si>
+    <t>As a petowner, Given that I have posted a job, I can view and modify its details.</t>
+  </si>
+  <si>
+    <t>As a petowner, Given that I have posted a job, I can delete it.</t>
+  </si>
+  <si>
+    <t>As a petowner, Given that I have posted a job, I can see the pet sitters that applied.</t>
+  </si>
+  <si>
+    <t>As a petowner, Given that I have found a suitable candidate, I can approve them.</t>
+  </si>
+  <si>
+    <t>As a petowner, I can modify my account details.</t>
+  </si>
+  <si>
+    <t>As a petowner, I can delete my account.</t>
+  </si>
+  <si>
+    <t>As a petsitter, I can view a list of pets that need looking after.</t>
+  </si>
+  <si>
+    <t>As a petsitter, Given that I have found a job, I can apply for it.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,8 +261,37 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF262626"/>
+      <name val="NewBaskerville-Roman"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFCCA659"/>
+      <name val="Wingdings2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="NewBaskerville-Bold"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="NewBaskerville-Bold"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -146,8 +304,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -263,11 +433,186 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -299,11 +644,274 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF262626"/>
+        <name val="NewBaskerville-Roman"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF262626"/>
+        <name val="NewBaskerville-Roman"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -314,6 +922,30 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{57C5B3FA-5D07-4CF9-A8AB-5593494AC4E8}" name="Таблица2" displayName="Таблица2" ref="B2:D18" totalsRowShown="0" headerRowDxfId="9" tableBorderDxfId="8">
+  <autoFilter ref="B2:D18" xr:uid="{C01B480D-C215-495C-AF64-2A4E4A32F445}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{2CF9606B-D7AE-4CF7-8843-0AFC9274C9EF}" name="#" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{15B93BF7-94A7-446B-A71E-F58358FFF5E0}" name="Story description" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{72D7DB73-E701-4423-9E2C-0A9669828FE9}" name="Selected to realize" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CE337D6C-4DE6-4F29-98F6-863284413C59}" name="Таблица3" displayName="Таблица3" ref="B20:D37" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5">
+  <autoFilter ref="B20:D37" xr:uid="{6CFEE017-7BE5-405F-9423-A347C79528E5}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{A6B59A8E-45DB-4C05-8125-53F84A89D926}" name="#" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{982DEC9F-FB01-4425-BB6C-2F48BB6E3F4A}" name="Story description" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{E3C3D523-F500-4069-8BCB-128ADD99D757}" name="Selected to realize" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -615,23 +1247,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A36D8BA7-1B6B-41A3-B7AE-6C59322D3D25}">
   <dimension ref="B2:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="31.85546875" customWidth="1"/>
     <col min="3" max="3" width="54.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" ht="19.5" customHeight="1">
       <c r="B2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:3" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" ht="15.75" thickBot="1"/>
+    <row r="4" spans="2:3" ht="27.75" customHeight="1" thickBot="1">
       <c r="B4" s="13" t="s">
         <v>14</v>
       </c>
@@ -639,11 +1271,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3">
       <c r="B5" s="5"/>
       <c r="C5" s="7"/>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3">
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
@@ -651,11 +1283,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3">
       <c r="B7" s="1"/>
       <c r="C7" s="8"/>
     </row>
-    <row r="8" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" ht="45">
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
@@ -663,11 +1295,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3">
       <c r="B9" s="1"/>
       <c r="C9" s="8"/>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3">
       <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
@@ -675,7 +1307,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" ht="15.75" thickBot="1">
       <c r="B11" s="3"/>
       <c r="C11" s="9"/>
     </row>
@@ -686,27 +1318,489 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AE8DDA7-B67D-4EAA-8AB5-0744582868C8}">
-  <dimension ref="B2:D19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{353ED11B-5486-4595-83EF-5512B870E63C}">
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="84.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75" customHeight="1" thickBot="1"/>
+    <row r="2" spans="1:4" ht="39" customHeight="1">
+      <c r="A2" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="27">
+        <v>1</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="40"/>
+      <c r="B4" s="27">
+        <v>2</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="26.25">
+      <c r="A5" s="40"/>
+      <c r="B5" s="27">
+        <v>3</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="40"/>
+      <c r="B6" s="27">
+        <v>4</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="40"/>
+      <c r="B7" s="27">
+        <v>5</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="40"/>
+      <c r="B8" s="27">
+        <v>6</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="40"/>
+      <c r="B9" s="27">
+        <v>7</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="40"/>
+      <c r="B10" s="27">
+        <v>8</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="40"/>
+      <c r="B11" s="27">
+        <v>9</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="40"/>
+      <c r="B12" s="27">
+        <v>10</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="40"/>
+      <c r="B13" s="27">
+        <v>11</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="40"/>
+      <c r="B14" s="27">
+        <v>12</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="40"/>
+      <c r="B15" s="27">
+        <v>13</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="40"/>
+      <c r="B16" s="27">
+        <v>14</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="40"/>
+      <c r="B17" s="27">
+        <v>15</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="41"/>
+      <c r="B18" s="28">
+        <v>16</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C19" s="17"/>
+    </row>
+    <row r="20" spans="1:4" ht="33" customHeight="1">
+      <c r="A20" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="37" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="27">
+        <v>1</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="40"/>
+      <c r="B22" s="27">
+        <v>2</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="40"/>
+      <c r="B23" s="27">
+        <v>3</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="40"/>
+      <c r="B24" s="27">
+        <v>4</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="26.25">
+      <c r="A25" s="40"/>
+      <c r="B25" s="27">
+        <v>5</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="40"/>
+      <c r="B26" s="27">
+        <v>6</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="40"/>
+      <c r="B27" s="27">
+        <v>7</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="40"/>
+      <c r="B28" s="27">
+        <v>8</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="40"/>
+      <c r="B29" s="27">
+        <v>9</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="40"/>
+      <c r="B30" s="27">
+        <v>10</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="40"/>
+      <c r="B31" s="27">
+        <v>11</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="40"/>
+      <c r="B32" s="27">
+        <v>12</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="40"/>
+      <c r="B33" s="27">
+        <v>13</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="40"/>
+      <c r="B34" s="27">
+        <v>14</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="40"/>
+      <c r="B35" s="27">
+        <v>15</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D35" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="40"/>
+      <c r="B36" s="27">
+        <v>16</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D36" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="26.25">
+      <c r="A37" s="41"/>
+      <c r="B37" s="28">
+        <v>17</v>
+      </c>
+      <c r="C37" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:A18"/>
+    <mergeCell ref="A21:A37"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AE8DDA7-B67D-4EAA-8AB5-0744582868C8}">
+  <dimension ref="B2:D26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="30.5703125" customWidth="1"/>
     <col min="3" max="3" width="65.140625" customWidth="1"/>
     <col min="4" max="4" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" ht="15.75" thickBot="1"/>
+    <row r="4" spans="2:4" ht="33.75" customHeight="1" thickBot="1">
       <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
@@ -717,12 +1811,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4">
       <c r="B5" s="5"/>
       <c r="C5" s="7"/>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4">
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
@@ -733,12 +1827,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4">
       <c r="B7" s="1"/>
       <c r="C7" s="8"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4">
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -749,12 +1843,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4">
       <c r="B9" s="1"/>
       <c r="C9" s="8"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4">
       <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
@@ -765,12 +1859,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4">
       <c r="B11" s="1"/>
       <c r="C11" s="8"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4">
       <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
@@ -781,12 +1875,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4">
       <c r="B13" s="1"/>
       <c r="C13" s="8"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4">
       <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
@@ -797,12 +1891,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4">
       <c r="B15" s="1"/>
       <c r="C15" s="8"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4">
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
@@ -813,12 +1907,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4">
       <c r="B17" s="1"/>
       <c r="C17" s="8"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4">
       <c r="B18" s="1" t="s">
         <v>12</v>
       </c>
@@ -829,27 +1923,46 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" ht="15.75" thickBot="1">
       <c r="B19" s="3"/>
       <c r="C19" s="9"/>
       <c r="D19" s="4"/>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="15.75" thickBot="1"/>
+    <row r="24" spans="2:4">
+      <c r="B24" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" s="21"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="30"/>
+    </row>
+    <row r="26" spans="2:4" ht="15.75" thickBot="1">
+      <c r="B26" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" s="31" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{353ED11B-5486-4595-83EF-5512B870E63C}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Potential client errors list regard to PetSitter API endpoints.
</commit_message>
<xml_diff>
--- a/src/main/resources/PetSitter/RequirementsList.xlsx
+++ b/src/main/resources/PetSitter/RequirementsList.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jp\spring-boot-openapi\src\main\resources\PetSitter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19D9F0D-31E4-4ABD-B537-C72C7E5D0541}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0DAB6B-7DC4-4F54-8A50-03BAFCFD6D26}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-210" windowWidth="29040" windowHeight="15840" xr2:uid="{A9D3E40F-915C-4BF8-899F-BC9B8C8FC226}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{A9D3E40F-915C-4BF8-899F-BC9B8C8FC226}"/>
   </bookViews>
   <sheets>
     <sheet name="App user roles" sheetId="2" r:id="rId1"/>
     <sheet name="User Stories" sheetId="3" r:id="rId2"/>
     <sheet name="Requirements" sheetId="1" r:id="rId3"/>
+    <sheet name="Problem_json" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="93">
   <si>
     <t>Requirements list draft</t>
   </si>
@@ -231,6 +232,90 @@
   </si>
   <si>
     <t>As a petsitter, Given that I have found a job, I can apply for it.</t>
+  </si>
+  <si>
+    <t>Endpoint path</t>
+  </si>
+  <si>
+    <t>Problem description</t>
+  </si>
+  <si>
+    <t>POST /register</t>
+  </si>
+  <si>
+    <t>Mulformed input (no any JSON or invalid JSON), missing fields or invalid data types</t>
+  </si>
+  <si>
+    <t>User might be already exists</t>
+  </si>
+  <si>
+    <t>GET /users/{id}</t>
+  </si>
+  <si>
+    <t>User is not allowed to access to another user</t>
+  </si>
+  <si>
+    <t>PUT /user/{id}</t>
+  </si>
+  <si>
+    <t>DELETE /user/{id}</t>
+  </si>
+  <si>
+    <t>User does not exist</t>
+  </si>
+  <si>
+    <t>POST /jobs</t>
+  </si>
+  <si>
+    <t>User is not allowed to created a new job since they don not have the "Pet Sitter" app role</t>
+  </si>
+  <si>
+    <t>GET /jobs</t>
+  </si>
+  <si>
+    <t>Invalid input for the query parameters (e.g. invalid filters, pagination, or sorting)</t>
+  </si>
+  <si>
+    <t>GET /jobs/{id}</t>
+  </si>
+  <si>
+    <t>Job does not exist</t>
+  </si>
+  <si>
+    <t>PUT /jobs/{id}</t>
+  </si>
+  <si>
+    <t>User is now allowed to modified to modify the job, and they are not an admin app role</t>
+  </si>
+  <si>
+    <t>DELETE /jobs/{id}</t>
+  </si>
+  <si>
+    <t>POST /jobs/{id}/jobs-applications</t>
+  </si>
+  <si>
+    <t>GET /jobs/{id}/job-applications</t>
+  </si>
+  <si>
+    <t>GET /users/{id}/jobs</t>
+  </si>
+  <si>
+    <t>PUT /job-applications/{id}</t>
+  </si>
+  <si>
+    <t>Job application does not exist</t>
+  </si>
+  <si>
+    <t>User is not allowed to modify the job application</t>
+  </si>
+  <si>
+    <t>POST /sessions</t>
+  </si>
+  <si>
+    <t>Invalid credentials</t>
+  </si>
+  <si>
+    <t>Is included ?</t>
   </si>
 </sst>
 </file>
@@ -241,14 +326,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -290,6 +367,13 @@
       <color rgb="FF000000"/>
       <name val="NewBaskerville-Bold"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -317,7 +401,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -608,11 +692,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -623,16 +722,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -644,18 +737,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -673,20 +766,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -697,30 +793,31 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="13">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -733,25 +830,20 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF262626"/>
-        <name val="NewBaskerville-Roman"/>
+        <sz val="16"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
         <scheme val="none"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -855,6 +947,54 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF262626"/>
+        <name val="NewBaskerville-Roman"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -925,24 +1065,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{57C5B3FA-5D07-4CF9-A8AB-5593494AC4E8}" name="Таблица2" displayName="Таблица2" ref="B2:D18" totalsRowShown="0" headerRowDxfId="9" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{57C5B3FA-5D07-4CF9-A8AB-5593494AC4E8}" name="Таблица2" displayName="Таблица2" ref="B2:D18" totalsRowShown="0" headerRowDxfId="12" tableBorderDxfId="11">
   <autoFilter ref="B2:D18" xr:uid="{C01B480D-C215-495C-AF64-2A4E4A32F445}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{2CF9606B-D7AE-4CF7-8843-0AFC9274C9EF}" name="#" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{15B93BF7-94A7-446B-A71E-F58358FFF5E0}" name="Story description" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{72D7DB73-E701-4423-9E2C-0A9669828FE9}" name="Selected to realize" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{2CF9606B-D7AE-4CF7-8843-0AFC9274C9EF}" name="#" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{15B93BF7-94A7-446B-A71E-F58358FFF5E0}" name="Story description" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{72D7DB73-E701-4423-9E2C-0A9669828FE9}" name="Selected to realize" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CE337D6C-4DE6-4F29-98F6-863284413C59}" name="Таблица3" displayName="Таблица3" ref="B20:D37" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CE337D6C-4DE6-4F29-98F6-863284413C59}" name="Таблица3" displayName="Таблица3" ref="B20:D37" totalsRowShown="0" headerRowDxfId="7" tableBorderDxfId="6">
   <autoFilter ref="B20:D37" xr:uid="{6CFEE017-7BE5-405F-9423-A347C79528E5}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{A6B59A8E-45DB-4C05-8125-53F84A89D926}" name="#" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{982DEC9F-FB01-4425-BB6C-2F48BB6E3F4A}" name="Story description" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{E3C3D523-F500-4069-8BCB-128ADD99D757}" name="Selected to realize" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{A6B59A8E-45DB-4C05-8125-53F84A89D926}" name="#" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{982DEC9F-FB01-4425-BB6C-2F48BB6E3F4A}" name="Story description" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{E3C3D523-F500-4069-8BCB-128ADD99D757}" name="Selected to realize" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BA1139A9-F575-48AE-B605-4F8737F0E051}" name="Таблица6" displayName="Таблица6" ref="B4:D51" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="B4:D51" xr:uid="{0840EFDE-9D2A-460C-9078-F793B97A20BD}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{65AF4D72-6B01-42ED-83CB-3E418578EFAA}" name="Endpoint path" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{163E1125-4CCD-4B7A-90E9-A0B54FA0837A}" name="Problem description" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{E9DD0F1C-F947-4763-8904-2FD768F290D4}" name="Is included ?"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1247,8 +1399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A36D8BA7-1B6B-41A3-B7AE-6C59322D3D25}">
   <dimension ref="B2:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1264,10 +1416,10 @@
     </row>
     <row r="3" spans="2:3" ht="15.75" thickBot="1"/>
     <row r="4" spans="2:3" ht="27.75" customHeight="1" thickBot="1">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="42" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1291,7 +1443,7 @@
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="13" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1321,8 +1473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{353ED11B-5486-4595-83EF-5512B870E63C}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1335,433 +1487,433 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" customHeight="1" thickBot="1"/>
     <row r="2" spans="1:4" ht="39" customHeight="1">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="35" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="27">
+      <c r="B3" s="25">
         <v>1</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="40"/>
-      <c r="B4" s="27">
+      <c r="A4" s="39"/>
+      <c r="B4" s="25">
         <v>2</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="26.25">
-      <c r="A5" s="40"/>
-      <c r="B5" s="27">
+      <c r="A5" s="39"/>
+      <c r="B5" s="25">
         <v>3</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="40"/>
-      <c r="B6" s="27">
+      <c r="A6" s="39"/>
+      <c r="B6" s="25">
         <v>4</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="40"/>
-      <c r="B7" s="27">
+      <c r="A7" s="39"/>
+      <c r="B7" s="25">
         <v>5</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="42" t="s">
+      <c r="D7" s="37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="40"/>
-      <c r="B8" s="27">
+      <c r="A8" s="39"/>
+      <c r="B8" s="25">
         <v>6</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="40"/>
-      <c r="B9" s="27">
+      <c r="A9" s="39"/>
+      <c r="B9" s="25">
         <v>7</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="40"/>
-      <c r="B10" s="27">
+      <c r="A10" s="39"/>
+      <c r="B10" s="25">
         <v>8</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="40"/>
-      <c r="B11" s="27">
+      <c r="A11" s="39"/>
+      <c r="B11" s="25">
         <v>9</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="40"/>
-      <c r="B12" s="27">
+      <c r="A12" s="39"/>
+      <c r="B12" s="25">
         <v>10</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="40"/>
-      <c r="B13" s="27">
+      <c r="A13" s="39"/>
+      <c r="B13" s="25">
         <v>11</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="42" t="s">
+      <c r="D13" s="37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="40"/>
-      <c r="B14" s="27">
+      <c r="A14" s="39"/>
+      <c r="B14" s="25">
         <v>12</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="40"/>
-      <c r="B15" s="27">
+      <c r="A15" s="39"/>
+      <c r="B15" s="25">
         <v>13</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="40"/>
-      <c r="B16" s="27">
+      <c r="A16" s="39"/>
+      <c r="B16" s="25">
         <v>14</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="42" t="s">
+      <c r="D16" s="37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="40"/>
-      <c r="B17" s="27">
+      <c r="A17" s="39"/>
+      <c r="B17" s="25">
         <v>15</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="42" t="s">
+      <c r="D17" s="37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="41"/>
-      <c r="B18" s="28">
+      <c r="A18" s="40"/>
+      <c r="B18" s="26">
         <v>16</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="42" t="s">
+      <c r="D18" s="37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" thickBot="1">
-      <c r="C19" s="17"/>
+      <c r="C19" s="15"/>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="37" t="s">
+      <c r="D20" s="35" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="27">
+      <c r="B21" s="25">
         <v>1</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="42" t="s">
+      <c r="D21" s="37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="40"/>
-      <c r="B22" s="27">
+      <c r="A22" s="39"/>
+      <c r="B22" s="25">
         <v>2</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="42" t="s">
+      <c r="D22" s="37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="40"/>
-      <c r="B23" s="27">
+      <c r="A23" s="39"/>
+      <c r="B23" s="25">
         <v>3</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="42" t="s">
+      <c r="D23" s="37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="40"/>
-      <c r="B24" s="27">
+      <c r="A24" s="39"/>
+      <c r="B24" s="25">
         <v>4</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="42" t="s">
+      <c r="D24" s="37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26.25">
-      <c r="A25" s="40"/>
-      <c r="B25" s="27">
+      <c r="A25" s="39"/>
+      <c r="B25" s="25">
         <v>5</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="C25" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="42" t="s">
+      <c r="D25" s="37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="40"/>
-      <c r="B26" s="27">
+      <c r="A26" s="39"/>
+      <c r="B26" s="25">
         <v>6</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="42" t="s">
+      <c r="D26" s="37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="40"/>
-      <c r="B27" s="27">
+      <c r="A27" s="39"/>
+      <c r="B27" s="25">
         <v>7</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="42" t="s">
+      <c r="D27" s="37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="40"/>
-      <c r="B28" s="27">
+      <c r="A28" s="39"/>
+      <c r="B28" s="25">
         <v>8</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D28" s="42" t="s">
+      <c r="D28" s="37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="40"/>
-      <c r="B29" s="27">
+      <c r="A29" s="39"/>
+      <c r="B29" s="25">
         <v>9</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="42" t="s">
+      <c r="D29" s="37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="40"/>
-      <c r="B30" s="27">
+      <c r="A30" s="39"/>
+      <c r="B30" s="25">
         <v>10</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="42" t="s">
+      <c r="D30" s="37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="40"/>
-      <c r="B31" s="27">
+      <c r="A31" s="39"/>
+      <c r="B31" s="25">
         <v>11</v>
       </c>
-      <c r="C31" s="18" t="s">
+      <c r="C31" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="42" t="s">
+      <c r="D31" s="37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="40"/>
-      <c r="B32" s="27">
+      <c r="A32" s="39"/>
+      <c r="B32" s="25">
         <v>12</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="42" t="s">
+      <c r="D32" s="37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="40"/>
-      <c r="B33" s="27">
+      <c r="A33" s="39"/>
+      <c r="B33" s="25">
         <v>13</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C33" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="42" t="s">
+      <c r="D33" s="37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="40"/>
-      <c r="B34" s="27">
+      <c r="A34" s="39"/>
+      <c r="B34" s="25">
         <v>14</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D34" s="42" t="s">
+      <c r="D34" s="37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="40"/>
-      <c r="B35" s="27">
+      <c r="A35" s="39"/>
+      <c r="B35" s="25">
         <v>15</v>
       </c>
-      <c r="C35" s="18" t="s">
+      <c r="C35" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D35" s="42" t="s">
+      <c r="D35" s="37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="40"/>
-      <c r="B36" s="27">
+      <c r="A36" s="39"/>
+      <c r="B36" s="25">
         <v>16</v>
       </c>
-      <c r="C36" s="18" t="s">
+      <c r="C36" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="D36" s="42" t="s">
+      <c r="D36" s="37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="26.25">
-      <c r="A37" s="41"/>
-      <c r="B37" s="28">
+      <c r="A37" s="40"/>
+      <c r="B37" s="26">
         <v>17</v>
       </c>
-      <c r="C37" s="38" t="s">
+      <c r="C37" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="D37" s="42" t="s">
+      <c r="D37" s="37" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1784,7 +1936,7 @@
   <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1823,7 +1975,7 @@
       <c r="C6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="14" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1839,7 +1991,7 @@
       <c r="C8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="14" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1855,7 +2007,7 @@
       <c r="C10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="14" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1871,7 +2023,7 @@
       <c r="C12" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="14" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1887,7 +2039,7 @@
       <c r="C14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="14" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1903,7 +2055,7 @@
       <c r="C16" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="14" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1919,7 +2071,7 @@
       <c r="C18" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="14" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1935,29 +2087,29 @@
     </row>
     <row r="23" spans="2:4" ht="15.75" thickBot="1"/>
     <row r="24" spans="2:4">
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="29" t="s">
+      <c r="D24" s="27" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="25" spans="2:4">
-      <c r="B25" s="21"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="30"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="28"/>
     </row>
     <row r="26" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="25" t="s">
+      <c r="C26" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="31" t="s">
+      <c r="D26" s="29" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1965,4 +2117,313 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A670AA7D-E34E-44A6-88A9-77F038FA4DBE}">
+  <dimension ref="B4:D51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="53.42578125" customWidth="1"/>
+    <col min="3" max="3" width="113.5703125" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:4" ht="31.5" customHeight="1">
+      <c r="B4" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="43" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="44"/>
+      <c r="C7" s="44" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="44" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" s="44"/>
+      <c r="C10" s="44" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="44" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" s="44"/>
+      <c r="C13" s="44" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" s="44"/>
+      <c r="C14" s="44" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" s="44"/>
+      <c r="C15" s="44"/>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="44" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" s="44"/>
+      <c r="C17" s="44" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="44" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20" s="44"/>
+      <c r="C20" s="44" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="B21" s="44"/>
+      <c r="C21" s="44"/>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="44" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="B24" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="44" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" s="44"/>
+      <c r="C25" s="44"/>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="B26" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="44" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="B27" s="44"/>
+      <c r="C27" s="44" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3">
+      <c r="B28" s="44"/>
+      <c r="C28" s="44" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3">
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+    </row>
+    <row r="30" spans="2:3">
+      <c r="B30" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="44" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="B31" s="44"/>
+      <c r="C31" s="44" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3">
+      <c r="B32" s="44"/>
+      <c r="C32" s="44"/>
+    </row>
+    <row r="33" spans="2:3">
+      <c r="B33" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="44" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3">
+      <c r="B34" s="44"/>
+      <c r="C34" s="44"/>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35" s="44" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3">
+      <c r="B36" s="44"/>
+      <c r="C36" s="44" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3">
+      <c r="B37" s="44"/>
+      <c r="C37" s="44" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3">
+      <c r="B38" s="44"/>
+      <c r="C38" s="44"/>
+    </row>
+    <row r="39" spans="2:3">
+      <c r="B39" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39" s="44" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3">
+      <c r="B40" s="44"/>
+      <c r="C40" s="44" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3">
+      <c r="B41" s="44"/>
+      <c r="C41" s="44"/>
+    </row>
+    <row r="42" spans="2:3">
+      <c r="B42" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="C42" s="44" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3">
+      <c r="B43" s="44"/>
+      <c r="C43" s="44" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3">
+      <c r="B44" s="44"/>
+      <c r="C44" s="44" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3">
+      <c r="B45" s="44"/>
+      <c r="C45" s="44"/>
+    </row>
+    <row r="46" spans="2:3">
+      <c r="B46" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" s="45" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3">
+      <c r="B47" s="44"/>
+      <c r="C47" s="44" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3">
+      <c r="B48" s="44"/>
+      <c r="C48" s="44"/>
+    </row>
+    <row r="49" spans="2:3">
+      <c r="B49" s="44"/>
+      <c r="C49" s="44"/>
+    </row>
+    <row r="50" spans="2:3">
+      <c r="B50" s="44"/>
+      <c r="C50" s="44"/>
+    </row>
+    <row r="51" spans="2:3">
+      <c r="B51" s="44"/>
+      <c r="C51" s="44"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Problem+json description added to RequirementsList.xlsx
</commit_message>
<xml_diff>
--- a/src/main/resources/PetSitter/RequirementsList.xlsx
+++ b/src/main/resources/PetSitter/RequirementsList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jp\spring-boot-openapi\src\main\resources\PetSitter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0DAB6B-7DC4-4F54-8A50-03BAFCFD6D26}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326A518C-F807-41A6-8533-298B115D38FE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{A9D3E40F-915C-4BF8-899F-BC9B8C8FC226}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="User Stories" sheetId="3" r:id="rId2"/>
     <sheet name="Requirements" sheetId="1" r:id="rId3"/>
     <sheet name="Problem_json" sheetId="4" r:id="rId4"/>
+    <sheet name="Лист1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="102">
   <si>
     <t>Requirements list draft</t>
   </si>
@@ -316,6 +317,33 @@
   </si>
   <si>
     <t>Is included ?</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>401</t>
+  </si>
+  <si>
+    <t>403</t>
+  </si>
+  <si>
+    <t>404</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Not Found</t>
+  </si>
+  <si>
+    <t>Access forbidden</t>
+  </si>
+  <si>
+    <t>Unauthorized</t>
+  </si>
+  <si>
+    <t>Bad Request</t>
   </si>
 </sst>
 </file>
@@ -784,15 +812,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -807,6 +826,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1089,12 +1117,16 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BA1139A9-F575-48AE-B605-4F8737F0E051}" name="Таблица6" displayName="Таблица6" ref="B4:D51" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="B4:D51" xr:uid="{0840EFDE-9D2A-460C-9078-F793B97A20BD}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BA1139A9-F575-48AE-B605-4F8737F0E051}" name="Таблица6" displayName="Таблица6" ref="B4:H48" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="B4:H48" xr:uid="{0840EFDE-9D2A-460C-9078-F793B97A20BD}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{65AF4D72-6B01-42ED-83CB-3E418578EFAA}" name="Endpoint path" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{163E1125-4CCD-4B7A-90E9-A0B54FA0837A}" name="Problem description" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{E9DD0F1C-F947-4763-8904-2FD768F290D4}" name="Is included ?"/>
+    <tableColumn id="4" xr3:uid="{873C688F-43F1-4C08-BAE2-EED45997A9A1}" name="400"/>
+    <tableColumn id="5" xr3:uid="{5BB2A23B-EDF0-4EEC-81C4-A8D99390EE96}" name="401"/>
+    <tableColumn id="6" xr3:uid="{A0C0DCFA-EA84-474F-B43B-86CB1472921C}" name="403"/>
+    <tableColumn id="7" xr3:uid="{7137C5C3-CD63-4B53-A85A-2FC21BA85BE0}" name="404"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1416,10 +1448,10 @@
     </row>
     <row r="3" spans="2:3" ht="15.75" thickBot="1"/>
     <row r="4" spans="2:3" ht="27.75" customHeight="1" thickBot="1">
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="39" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1501,7 +1533,7 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="43" t="s">
         <v>46</v>
       </c>
       <c r="B3" s="25">
@@ -1515,7 +1547,7 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="39"/>
+      <c r="A4" s="44"/>
       <c r="B4" s="25">
         <v>2</v>
       </c>
@@ -1527,7 +1559,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="26.25">
-      <c r="A5" s="39"/>
+      <c r="A5" s="44"/>
       <c r="B5" s="25">
         <v>3</v>
       </c>
@@ -1539,7 +1571,7 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="39"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="25">
         <v>4</v>
       </c>
@@ -1551,7 +1583,7 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="39"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="25">
         <v>5</v>
       </c>
@@ -1563,7 +1595,7 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="39"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="25">
         <v>6</v>
       </c>
@@ -1575,7 +1607,7 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="39"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="25">
         <v>7</v>
       </c>
@@ -1587,7 +1619,7 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="39"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="25">
         <v>8</v>
       </c>
@@ -1599,7 +1631,7 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="39"/>
+      <c r="A11" s="44"/>
       <c r="B11" s="25">
         <v>9</v>
       </c>
@@ -1611,7 +1643,7 @@
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="39"/>
+      <c r="A12" s="44"/>
       <c r="B12" s="25">
         <v>10</v>
       </c>
@@ -1623,7 +1655,7 @@
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="39"/>
+      <c r="A13" s="44"/>
       <c r="B13" s="25">
         <v>11</v>
       </c>
@@ -1635,7 +1667,7 @@
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="39"/>
+      <c r="A14" s="44"/>
       <c r="B14" s="25">
         <v>12</v>
       </c>
@@ -1647,7 +1679,7 @@
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="39"/>
+      <c r="A15" s="44"/>
       <c r="B15" s="25">
         <v>13</v>
       </c>
@@ -1659,7 +1691,7 @@
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="39"/>
+      <c r="A16" s="44"/>
       <c r="B16" s="25">
         <v>14</v>
       </c>
@@ -1671,7 +1703,7 @@
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="39"/>
+      <c r="A17" s="44"/>
       <c r="B17" s="25">
         <v>15</v>
       </c>
@@ -1683,7 +1715,7 @@
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="40"/>
+      <c r="A18" s="45"/>
       <c r="B18" s="26">
         <v>16</v>
       </c>
@@ -1712,7 +1744,7 @@
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="38" t="s">
+      <c r="A21" s="43" t="s">
         <v>41</v>
       </c>
       <c r="B21" s="25">
@@ -1726,7 +1758,7 @@
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="39"/>
+      <c r="A22" s="44"/>
       <c r="B22" s="25">
         <v>2</v>
       </c>
@@ -1738,7 +1770,7 @@
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="39"/>
+      <c r="A23" s="44"/>
       <c r="B23" s="25">
         <v>3</v>
       </c>
@@ -1750,7 +1782,7 @@
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="39"/>
+      <c r="A24" s="44"/>
       <c r="B24" s="25">
         <v>4</v>
       </c>
@@ -1762,7 +1794,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="26.25">
-      <c r="A25" s="39"/>
+      <c r="A25" s="44"/>
       <c r="B25" s="25">
         <v>5</v>
       </c>
@@ -1774,7 +1806,7 @@
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="39"/>
+      <c r="A26" s="44"/>
       <c r="B26" s="25">
         <v>6</v>
       </c>
@@ -1786,7 +1818,7 @@
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="39"/>
+      <c r="A27" s="44"/>
       <c r="B27" s="25">
         <v>7</v>
       </c>
@@ -1798,7 +1830,7 @@
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="39"/>
+      <c r="A28" s="44"/>
       <c r="B28" s="25">
         <v>8</v>
       </c>
@@ -1810,7 +1842,7 @@
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="39"/>
+      <c r="A29" s="44"/>
       <c r="B29" s="25">
         <v>9</v>
       </c>
@@ -1822,7 +1854,7 @@
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="39"/>
+      <c r="A30" s="44"/>
       <c r="B30" s="25">
         <v>10</v>
       </c>
@@ -1834,7 +1866,7 @@
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="39"/>
+      <c r="A31" s="44"/>
       <c r="B31" s="25">
         <v>11</v>
       </c>
@@ -1846,7 +1878,7 @@
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="39"/>
+      <c r="A32" s="44"/>
       <c r="B32" s="25">
         <v>12</v>
       </c>
@@ -1858,7 +1890,7 @@
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="39"/>
+      <c r="A33" s="44"/>
       <c r="B33" s="25">
         <v>13</v>
       </c>
@@ -1870,7 +1902,7 @@
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="39"/>
+      <c r="A34" s="44"/>
       <c r="B34" s="25">
         <v>14</v>
       </c>
@@ -1882,7 +1914,7 @@
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="39"/>
+      <c r="A35" s="44"/>
       <c r="B35" s="25">
         <v>15</v>
       </c>
@@ -1894,7 +1926,7 @@
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="39"/>
+      <c r="A36" s="44"/>
       <c r="B36" s="25">
         <v>16</v>
       </c>
@@ -1906,7 +1938,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="26.25">
-      <c r="A37" s="40"/>
+      <c r="A37" s="45"/>
       <c r="B37" s="26">
         <v>17</v>
       </c>
@@ -2121,303 +2153,490 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A670AA7D-E34E-44A6-88A9-77F038FA4DBE}">
-  <dimension ref="B4:D51"/>
+  <dimension ref="B3:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="5.5703125" customWidth="1"/>
     <col min="2" max="2" width="53.42578125" customWidth="1"/>
-    <col min="3" max="3" width="113.5703125" customWidth="1"/>
-    <col min="4" max="4" width="37.42578125" customWidth="1"/>
+    <col min="3" max="3" width="93.140625" customWidth="1"/>
+    <col min="4" max="4" width="30" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:4" ht="31.5" customHeight="1">
-      <c r="B4" s="43" t="s">
+    <row r="3" spans="2:8">
+      <c r="E3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="31.5" customHeight="1">
+      <c r="B4" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="43" t="s">
+      <c r="C4" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="43" t="s">
+      <c r="D4" s="40" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="5" spans="2:4">
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-    </row>
-    <row r="6" spans="2:4">
-      <c r="B6" s="44" t="s">
+      <c r="E4" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="G4" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" s="40" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="B6" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="41" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="7" spans="2:4">
-      <c r="B7" s="44"/>
-      <c r="C7" s="44" t="s">
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="B7" s="41"/>
+      <c r="C7" s="41" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="2:4">
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
-    </row>
-    <row r="9" spans="2:4">
-      <c r="B9" s="44" t="s">
+    <row r="8" spans="2:8">
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="B9" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="41" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="10" spans="2:4">
-      <c r="B10" s="44"/>
-      <c r="C10" s="44" t="s">
+      <c r="E9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="B10" s="41"/>
+      <c r="C10" s="41" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="2:4">
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
-    </row>
-    <row r="12" spans="2:4">
-      <c r="B12" s="44" t="s">
+    <row r="11" spans="2:8">
+      <c r="B11" s="41"/>
+      <c r="C11" s="41"/>
+    </row>
+    <row r="12" spans="2:8">
+      <c r="B12" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="44" t="s">
+      <c r="C12" s="41" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="13" spans="2:4">
-      <c r="B13" s="44"/>
-      <c r="C13" s="44" t="s">
+      <c r="E12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8">
+      <c r="B13" s="41"/>
+      <c r="C13" s="41" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="2:4">
-      <c r="B14" s="44"/>
-      <c r="C14" s="44" t="s">
+    <row r="14" spans="2:8">
+      <c r="B14" s="41"/>
+      <c r="C14" s="41" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="2:4">
-      <c r="B15" s="44"/>
-      <c r="C15" s="44"/>
-    </row>
-    <row r="16" spans="2:4">
-      <c r="B16" s="44" t="s">
+    <row r="15" spans="2:8">
+      <c r="B15" s="41"/>
+      <c r="C15" s="41"/>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="B16" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="C16" s="44" t="s">
+      <c r="C16" s="41" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="17" spans="2:3">
-      <c r="B17" s="44"/>
-      <c r="C17" s="44" t="s">
+      <c r="E16" t="s">
+        <v>97</v>
+      </c>
+      <c r="F16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" s="41"/>
+      <c r="C17" s="41" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
-      <c r="B18" s="44"/>
-      <c r="C18" s="44"/>
-    </row>
-    <row r="19" spans="2:3">
-      <c r="B19" s="44" t="s">
+    <row r="18" spans="2:8">
+      <c r="B18" s="41"/>
+      <c r="C18" s="41"/>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="B19" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="44" t="s">
+      <c r="C19" s="41" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="20" spans="2:3">
-      <c r="B20" s="44"/>
-      <c r="C20" s="44" t="s">
+      <c r="E19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8">
+      <c r="B20" s="41"/>
+      <c r="C20" s="41" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
-      <c r="B21" s="44"/>
-      <c r="C21" s="44"/>
-    </row>
-    <row r="22" spans="2:3">
-      <c r="B22" s="44" t="s">
+    <row r="21" spans="2:8">
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
+    </row>
+    <row r="22" spans="2:8">
+      <c r="B22" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="C22" s="44" t="s">
+      <c r="C22" s="41" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="23" spans="2:3">
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
-    </row>
-    <row r="24" spans="2:3">
-      <c r="B24" s="44" t="s">
+      <c r="E22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" t="s">
+        <v>97</v>
+      </c>
+      <c r="H22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8">
+      <c r="B23" s="41"/>
+      <c r="C23" s="41"/>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="B24" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="C24" s="44" t="s">
+      <c r="C24" s="41" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="25" spans="2:3">
-      <c r="B25" s="44"/>
-      <c r="C25" s="44"/>
-    </row>
-    <row r="26" spans="2:3">
-      <c r="B26" s="44" t="s">
+      <c r="E24" t="s">
+        <v>97</v>
+      </c>
+      <c r="F24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" t="s">
+        <v>97</v>
+      </c>
+      <c r="H24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="B25" s="41"/>
+      <c r="C25" s="41"/>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="C26" s="44" t="s">
+      <c r="C26" s="41" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="27" spans="2:3">
-      <c r="B27" s="44"/>
-      <c r="C27" s="44" t="s">
+      <c r="E26" t="s">
+        <v>22</v>
+      </c>
+      <c r="F26" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="B27" s="41"/>
+      <c r="C27" s="41" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="2:3">
-      <c r="B28" s="44"/>
-      <c r="C28" s="44" t="s">
+    <row r="28" spans="2:8">
+      <c r="B28" s="41"/>
+      <c r="C28" s="41" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="2:3">
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-    </row>
-    <row r="30" spans="2:3">
-      <c r="B30" s="44" t="s">
+    <row r="29" spans="2:8">
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+    </row>
+    <row r="30" spans="2:8">
+      <c r="B30" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="C30" s="44" t="s">
+      <c r="C30" s="41" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="31" spans="2:3">
-      <c r="B31" s="44"/>
-      <c r="C31" s="44" t="s">
+      <c r="E30" t="s">
+        <v>97</v>
+      </c>
+      <c r="F30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G30" t="s">
+        <v>22</v>
+      </c>
+      <c r="H30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8">
+      <c r="B31" s="41"/>
+      <c r="C31" s="41" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="32" spans="2:3">
-      <c r="B32" s="44"/>
-      <c r="C32" s="44"/>
-    </row>
-    <row r="33" spans="2:3">
-      <c r="B33" s="44" t="s">
+    <row r="32" spans="2:8">
+      <c r="B32" s="41"/>
+      <c r="C32" s="41"/>
+    </row>
+    <row r="33" spans="2:8">
+      <c r="B33" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="C33" s="44" t="s">
+      <c r="C33" s="41" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="34" spans="2:3">
-      <c r="B34" s="44"/>
-      <c r="C34" s="44"/>
-    </row>
-    <row r="35" spans="2:3">
-      <c r="B35" s="44" t="s">
+      <c r="E33" t="s">
+        <v>97</v>
+      </c>
+      <c r="F33" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33" t="s">
+        <v>22</v>
+      </c>
+      <c r="H33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8">
+      <c r="B34" s="41"/>
+      <c r="C34" s="41"/>
+    </row>
+    <row r="35" spans="2:8">
+      <c r="B35" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="C35" s="44" t="s">
+      <c r="C35" s="41" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="36" spans="2:3">
-      <c r="B36" s="44"/>
-      <c r="C36" s="44" t="s">
+      <c r="E35" t="s">
+        <v>22</v>
+      </c>
+      <c r="F35" t="s">
+        <v>22</v>
+      </c>
+      <c r="G35" t="s">
+        <v>22</v>
+      </c>
+      <c r="H35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8">
+      <c r="B36" s="41"/>
+      <c r="C36" s="41" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="2:3">
-      <c r="B37" s="44"/>
-      <c r="C37" s="44" t="s">
+    <row r="37" spans="2:8">
+      <c r="B37" s="41"/>
+      <c r="C37" s="41" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="2:3">
-      <c r="B38" s="44"/>
-      <c r="C38" s="44"/>
-    </row>
-    <row r="39" spans="2:3">
-      <c r="B39" s="44" t="s">
+    <row r="38" spans="2:8">
+      <c r="B38" s="41"/>
+      <c r="C38" s="41"/>
+    </row>
+    <row r="39" spans="2:8">
+      <c r="B39" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="C39" s="44" t="s">
+      <c r="C39" s="41" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="40" spans="2:3">
-      <c r="B40" s="44"/>
-      <c r="C40" s="44" t="s">
+      <c r="E39" t="s">
+        <v>97</v>
+      </c>
+      <c r="F39" t="s">
+        <v>22</v>
+      </c>
+      <c r="G39" t="s">
+        <v>22</v>
+      </c>
+      <c r="H39" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8">
+      <c r="B40" s="41"/>
+      <c r="C40" s="41" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="2:3">
-      <c r="B41" s="44"/>
-      <c r="C41" s="44"/>
-    </row>
-    <row r="42" spans="2:3">
-      <c r="B42" s="44" t="s">
+    <row r="41" spans="2:8">
+      <c r="B41" s="41"/>
+      <c r="C41" s="41"/>
+    </row>
+    <row r="42" spans="2:8">
+      <c r="B42" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="C42" s="44" t="s">
+      <c r="C42" s="41" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="43" spans="2:3">
-      <c r="B43" s="44"/>
-      <c r="C43" s="44" t="s">
+      <c r="E42" t="s">
+        <v>97</v>
+      </c>
+      <c r="F42" t="s">
+        <v>22</v>
+      </c>
+      <c r="G42" t="s">
+        <v>22</v>
+      </c>
+      <c r="H42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8">
+      <c r="B43" s="41"/>
+      <c r="C43" s="41" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="2:3">
-      <c r="B44" s="44"/>
-      <c r="C44" s="44" t="s">
+    <row r="44" spans="2:8">
+      <c r="B44" s="41"/>
+      <c r="C44" s="41" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="2:3">
-      <c r="B45" s="44"/>
-      <c r="C45" s="44"/>
-    </row>
-    <row r="46" spans="2:3">
-      <c r="B46" s="44" t="s">
+    <row r="45" spans="2:8">
+      <c r="B45" s="41"/>
+      <c r="C45" s="41"/>
+    </row>
+    <row r="46" spans="2:8">
+      <c r="B46" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="C46" s="45" t="s">
+      <c r="C46" s="42" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="47" spans="2:3">
-      <c r="B47" s="44"/>
-      <c r="C47" s="44" t="s">
+      <c r="E46" t="s">
+        <v>22</v>
+      </c>
+      <c r="F46" t="s">
+        <v>22</v>
+      </c>
+      <c r="G46" t="s">
+        <v>97</v>
+      </c>
+      <c r="H46" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8">
+      <c r="B47" s="41"/>
+      <c r="C47" s="41" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="2:3">
-      <c r="B48" s="44"/>
-      <c r="C48" s="44"/>
+    <row r="48" spans="2:8">
+      <c r="B48" s="41"/>
+      <c r="C48" s="41"/>
     </row>
     <row r="49" spans="2:3">
-      <c r="B49" s="44"/>
-      <c r="C49" s="44"/>
+      <c r="B49" s="41"/>
+      <c r="C49" s="41"/>
     </row>
     <row r="50" spans="2:3">
-      <c r="B50" s="44"/>
-      <c r="C50" s="44"/>
+      <c r="B50" s="41"/>
+      <c r="C50" s="41"/>
     </row>
     <row r="51" spans="2:3">
-      <c r="B51" s="44"/>
-      <c r="C51" s="44"/>
+      <c r="B51" s="41"/>
+      <c r="C51" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2426,4 +2645,16 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{327BADF5-F332-4919-98A3-762B2A8753F8}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>